<commit_message>
PQ Challenge 110 and Excel challenge 274 has been added.
</commit_message>
<xml_diff>
--- a/Excel Files/PQ Challenges/PQ Challenge 109 Problem.xlsx
+++ b/Excel Files/PQ Challenges/PQ Challenge 109 Problem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Excel-BI-Python\Excel Files\PQ Challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8429C6E2-9478-4FD8-A811-241200FC12B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F77F0D0-5520-4BAC-B230-B601F77AF644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -909,7 +909,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="1241" row="12">
+  <wetp:taskpane dockstate="right" visibility="0" width="1736" row="11">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -927,6 +927,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1003,7 +1006,7 @@
         <v>3</v>
       </c>
       <c r="J2" cm="1">
-        <f t="array" ref="J2:L5">_xlfn.LET(_xlpm.data, A2:C17, _xlpm.fxOne, _xlfn.LAMBDA(_xlpm.ForId, _xlfn.LET(_xlpm.FilteredData, _xlfn._xlws.FILTER(_xlpm.data, _xlfn.CHOOSECOLS(_xlpm.data, 1) = _xlpm.ForId), _xlpm.Seq, _xlfn.SEQUENCE(ROWS(_xlpm.FilteredData)), _xlpm.Mask, _xlfn.MAP(_xlpm.Seq, _xlfn.LAMBDA(_xlpm.RowIndex, IF(ISODD(_xlpm.RowIndex), AND(INDEX(_xlpm.FilteredData, _xlpm.RowIndex, 3) = "Entry", _xlpm.RowIndex &lt;&gt; ROWS(_xlpm.FilteredData)), INDEX(_xlpm.FilteredData, _xlpm.RowIndex, 3) = "Exit"))), _xlpm.Result, IFERROR(_xlfn._xlws.FILTER(_xlpm.FilteredData, NOT(_xlpm.Mask)), ""), _xlpm.Result)), _xlpm.Result, _xlfn.REDUCE("", _xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.data, 1)), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlpm.fxOne(_xlpm.v)))), _xlfn._xlws.FILTER(_xlpm.Result, _xlfn.CHOOSECOLS(_xlpm.Result, 1) &lt;&gt; ""))</f>
+        <f t="array" ref="J2:L5">_xlfn.LET(_xlpm.data, A2:C17, _xlpm.fxOne, _xlfn.LAMBDA(_xlpm.ForId, _xlfn.LET(_xlpm.FilteredData, _xlfn._xlws.FILTER(_xlpm.data, _xlfn.CHOOSECOLS(_xlpm.data, 1) = _xlpm.ForId), _xlpm.Seq, _xlfn.SEQUENCE(ROWS(_xlpm.FilteredData)), _xlpm.EntryRowsIndex, _xlfn._xlws.FILTER(_xlpm.Seq, INDEX(_xlpm.FilteredData, _xlpm.Seq, 3) = "Entry"), _xlpm.ValidExitRows, _xlfn._xlws.FILTER(_xlpm.EntryRowsIndex, IFERROR(INDEX(_xlpm.FilteredData, _xlpm.EntryRowsIndex + 1, 3) = "Exit", FALSE)), _xlpm.ValidRows, _xlfn.VSTACK(_xlpm.ValidExitRows, _xlpm.ValidExitRows + 1), _xlpm.IsInValidRows, MMULT(--(_xlpm.Seq = _xlfn.TOROW(_xlpm.ValidRows)), _xlfn.SEQUENCE(ROWS(_xlpm.ValidRows)) ^ 0) = 0, _xlpm.Result, IF(AND(ISERROR(_xlpm.ValidRows)), _xlpm.FilteredData, IFERROR(_xlfn._xlws.FILTER(_xlpm.FilteredData, _xlpm.IsInValidRows), "")), _xlpm.Result)), _xlpm.Result, _xlfn.REDUCE("", _xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.data, 1)), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlpm.fxOne(_xlpm.v)))), _xlpm.Final, _xlfn._xlws.FILTER(_xlpm.Result, _xlfn.CHOOSECOLS(_xlpm.Result, 1) &lt;&gt; ""), _xlpm.Final)</f>
         <v>1356</v>
       </c>
       <c r="K2">

</xml_diff>